<commit_message>
Fixed selector issues in job type search and adjusted clicks and types to simulate events.
</commit_message>
<xml_diff>
--- a/JHClientTarget.xlsx
+++ b/JHClientTarget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Programming\Revature\Revature UIPath Batch\Goldeneyez-P2\P2\Embrey_J\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B4B87E-E12C-4C77-B29D-1747DAA0F5B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82768DF-9FE1-4FE3-BFBB-BCC3EDE8612C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
     <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="0" activeTab="0" xr2:uid="{51044B34-69E7-4D1D-958A-13CEF9FD08F6}"/>
   </x:bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <x:si>
     <x:t>jobName</x:t>
   </x:si>
@@ -55,13 +55,13 @@
     <x:t>jobDescription</x:t>
   </x:si>
   <x:si>
-    <x:t>Senior Frontend Software Engineer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/partner/jobListing.htm?pos=101&amp;ao=1110586&amp;s=58&amp;guid=0000017cf3b55e24b00e722ac81ba86a&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;cs=1_0ec69475&amp;cb=1636176322882&amp;jobListingId=1007419377962&amp;cpc=46D02D9FC3E5D9C6&amp;jrtk=3-0-1fjpranobu4kr801-1fjpranp03oej000-f1d80eb8ab778cf2--6NYlbfkN0DDpz5gVDOkuskPWc7ZuaxPsWOyHj1g668dHwO5vI4Pl7wLnjdEKzJNZxrlMeC_-l2arzyFBV56WJEtYSSV_BU2WKWOgUnQrGGAutxW_iQc1VfZvFKZqfCaAz-DaUszDIs3hyyWPqK_MHSikdvReSLAmYVFS-PT_si91MyV_A_V78RXYRmu2VaHq6CHJrq3euDXaGVOqJSjaRfBaZrhmzhv1AHawfw8l3sZivJ1tC1PHmE-sVmTzQmGlX7NZWezDlCMzPEIjOCVDaKLP2wP1nMr_i8yFaiH63sNVQyNmg_wEPZlquXEkAN5DRS-cgK9wkWzXQCvcKAp7sG1y0pnzCQ3T42FHCYdaUlxhwlXYOJf_nowem_i086tRXEh0gpAij4nGvYmVU5bYNaA7bK8oG3neSuGusFXujxdw6yUqfIOOSV-AY3FV8I6rXN-WFid_LyDhbQFmjZkxhAaWTo0oS7nJRy4nRfHilcv2P71wvhbFpdRxrkiRP9lCz5L62FusbcykBrNSC2vYRkaXVwcxVtIO5v-fNThxWw%3D</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Dealerware</x:t>
+    <x:t>Senior Front-End Developer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/partner/jobListing.htm?pos=101&amp;ao=1110586&amp;s=58&amp;guid=0000017d01d12a9bb5752966b9d2839f&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=8F7263A855640A9C3D929937C67FB101&amp;ea=1&amp;cs=1_4995c90d&amp;cb=1636413025415&amp;jobListingId=1007380777928&amp;cpc=BD84E2634C97445A&amp;jrtk=3-0-1fk0t2ambu4um801-1fk0t2amou3mo800-791c059cda53df3b--6NYlbfkN0DAwgduWqBP7ymGN-lTADpinz2i-23XbRAyg5ywqS-MDRZJ25eGN4811vgchutyS2XszNTNJm9McZNVmsXi76R6GhBkV-aavNVJMFTUAfuj-vbdQvTYNAku0Kg-hHWNcNefQz1c95GXU2UQVJT9L_ZS0KbJ8TKNkHyswJoF-DxJGyLO_Yc2gepsB9x-62oWmVf22WY7rMmIhpURYE3tZWNK-I8RR0uBop4BSwV7hxg9hh5IACX0vT287zHSBxWDLh0fXIwhvkNkmYDy3TQOla6gB3Yxt_eUPRJqRNy8Bh4bbR2oN4v6gqGUcU2fQaVtb5tr3Lhb6MsMzXL_kHR3yAUuPnyDOCQJfevSxb-OdE1t4Y1awYZEEFkyJbzNCcLuTa6s1URfa86PujGGoWQ6nnOn7ELveyktDzNcSg6184nVZNPqUkeMRgr2J3m6-QOEL7GAOXyXkSUvBCz5SuYNXlYc9wLQsyJvjnLZR-hsfO_DocqWogSvQ7ibU9nlhYswGPA%3D</x:t>
+  </x:si>
+  <x:si>
+    <x:t>KIZEN Technologies, Inc.</x:t>
   </x:si>
   <x:si>
     <x:t>Austin, TX</x:t>
@@ -70,14 +70,13 @@
     <x:t xml:space="preserve"> Full-time</x:t>
   </x:si>
   <x:si>
-    <x:t>About Dealerware:
-Dealerware is modern fleet management for the modern retailer. We are proud to be ...</x:t>
+    <x:t>We are looking for a Senior Front-End Developer to join our rapidly growing team. This person will w...</x:t>
   </x:si>
   <x:si>
     <x:t>Software Engineering Senior Advisor</x:t>
   </x:si>
   <x:si>
-    <x:t>/partner/jobListing.htm?pos=102&amp;ao=1110586&amp;s=58&amp;guid=0000017cf3b55e24b00e722ac81ba86a&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;cs=1_8b39a185&amp;cb=1636176322883&amp;jobListingId=1007383667451&amp;cpc=96F8E6828E6A41D1&amp;jrtk=3-0-1fjpranobu4kr801-1fjpranp03oej000-9d4c55214232d9cd--6NYlbfkN0CJ4RVix5XbFvNEFGzeV6zdxykB_vlp8KSj_a_ovArNcpAUAf_1FZDHjCSGWhNpxUQMyoKTv9PM6XJueBvQ_5DfQXv_B9TQ5ZYRQ4CFNO3ggUgnV7IVmum8GxhrVOFwcxtXqXQ5sQdVkNfL_MK_SH3wf9qWbPfJnzDBPfD-S-Ev7zB7Kr5ZDZ0gH6D9kU3IC0YDwEl7rAlp_oM1HruYec08IR0LFjt4w21oHIL6kyCSZcPWvTZ2sjvZsdsCIIvHQIFrqDGZuBSz9LCpQm7-qnjea3LIhwV5eB0Rf-VrCBIilsPE21-lE9Vt1UXO3_vUEMdVzNybIJoryK5V8vCzqgFMlbqyo2YYVE93y6vI2XleWhc6Img2j7iYKsR0myYLw2dhQ_7shWvzGGoP2uqvFadOjTJHpvRbemlI9fspET5EOHK3xdMUCyk2wDo27_7mpuwo45aujvBDn86GM-8mKb2ClhOmuyRzcLlhp2v8aXRMXzrNFAKPIYZh-8Paw83sqTPKD05XUAgL05nS_xFJFqefvoLh2X3eCfdSxhC6zs0LfvwBZrvqCUS6</x:t>
+    <x:t>/partner/jobListing.htm?pos=102&amp;ao=1110586&amp;s=58&amp;guid=0000017d01d12a9bb5752966b9d2839f&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=8F7263A855640A9C3D929937C67FB101&amp;cs=1_1c288661&amp;cb=1636413025414&amp;jobListingId=1007383667451&amp;cpc=C05F74D5FBC032E7&amp;jrtk=3-0-1fk0t2ambu4um801-1fk0t2amou3mo800-9d4c55214232d9cd--6NYlbfkN0CJ4RVix5XbFvNEFGzeV6zdxykB_vlp8KSj_a_ovArNcpAUAf_1FZDHjCSGWhNpxUQMyoKTv9PM6XJueBvQ_5DfQXv_B9TQ5ZYRQ4CFNO3ggUgnV7IVmum8GxhrVOFwcxtXqXQ5sQdVkNfL_MK_SH3wf9qWbPfJnzDBPfD-S-Ev7zB7Kr5ZDZ0gbmqBOWG6DkdF7xL9CYWAfAwYhWqUETRvj_ER0R5zVFZC3ZfXPxf-BeynVuwDUGMbw2AzxzqV3YhK4IOzvtcQURMH361QcEkCEB0DK8jasPlno-6Ydvx1pgBnx7KegWDFyjKMNNTLGhUbwd3DAINr5LxRzlb0QBGTmmdecZgLUHL9DvgXA_shsnB0JtTP-Wz6Y4XTfT3uWmSojuyR9l_35HyFL5wFDjpngB3JV3orpSoqeF68oazK4K--CIiYOcD5hJzBZGbG8LNcWv1Idktf0a_XSDMA6pJj86wHIgnO1OMuyNJJaDHjORLuFOpQiyhTZLhDBLINshPEK0Sr-1KI7rRkbsCKTX4yFbZC6UC4y9cqCK4Z9LGd6Kr3PsPjUahj</x:t>
   </x:si>
   <x:si>
     <x:t>DirectSourcePRO</x:t>
@@ -90,96 +89,100 @@
 Ro...</x:t>
   </x:si>
   <x:si>
-    <x:t>Sr. Software Developer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/partner/jobListing.htm?pos=103&amp;ao=1110586&amp;s=58&amp;guid=0000017cf3b55e24b00e722ac81ba86a&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;ea=1&amp;cs=1_a128283b&amp;cb=1636176322885&amp;jobListingId=1007396037777&amp;cpc=3C7BB2D400054DDD&amp;jrtk=3-0-1fjpranobu4kr801-1fjpranp03oej000-00fe0bfa67468785--6NYlbfkN0Dl7F8yQ3Mt_M0p4pEaeq_LOWEMcxAwOSX3iRAQq_RxvjIAGLBwVtcuphiGOYMpONLNJY3tgQwuu1kqq9Z78oYeMqUfbrp_aouQSHE8ZDxGHRDqzG_6rK8PMatbavKOZ9j8KJFkeJi-Jk4E-hNU61jXBaxDfu-rszSIIaUuR3IDULzLZHe82xl2Hu4ybq7Cdfg8HTiSHA6GEt2NUJieeFfHONzP5cGjPmEQ_eRUZjK3EsEBkWsPnA9rJ_I_RJT2WlN76syzkbkd66eZtzSkT5mbl1CVhFRr0yi4VHFHqtwHBB4MONDpgcOvVQOlcCADcbxNunVD2-qDOomBog_r9mzSjVinz_1AeE1FrxdNNfBHMbL0RYvFx0L-7vJMN6dDFoXXBY6Rm0gimgyc9KJc7Mwkg7eIm3wjt1NwxYyBXeJ0gSj88PrVQ3Wyhs_XAHZx3ucmHsZW1GdShMhY78miuZOkryIskz8m93vg-LWcJ9SssC5dFvjqNS4T</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Resource Data</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Texas</x:t>
-  </x:si>
-  <x:si>
-    <x:t>You’ve proven your technical abilities are outstanding and you realize achieving results is more abo...</x:t>
+    <x:t>Software Engineer- Front End</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/partner/jobListing.htm?pos=103&amp;ao=1110586&amp;s=58&amp;guid=0000017d01d12a9bb5752966b9d2839f&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=8F7263A855640A9C3D929937C67FB101&amp;cs=1_4f0bc92c&amp;cb=1636413025414&amp;jobListingId=1007301089271&amp;cpc=61559BE6E921F6BF&amp;jrtk=3-0-1fk0t2ambu4um801-1fk0t2amou3mo800-123869a03d6bf7d7--6NYlbfkN0DeDTa8A5XXaP3hF5RUeGNUidlMB_lbQpEViSkLjPD18H4tnerHt4majvAAfyJrokiqScrhxLAgCS0vd18IfaNjzR2RXCQ125Q7hpl4vxXmeo3ZSHi_0NvGhcSiVfw-Ofy9vPkPzw9lMuZXyNTsqiPOA35x_zx1h7hSeuXVuhq7TINxJshxZu9ToXAhfCi5TliJvHHVD_T_khyVj2-AiC5to5RhpYqcz0sNYf-FwlEHOlISA-2f30PNVtn1IhRKvpvA5HIgjBcl5FPQF2tRjjp_cV4loVl85UnXccwbO9DBhM9ueeYpOi3NHdmOUprsbhqK5cmXQKC7XPFeJ1xn81kjUkh5d9YFAXTsLcC4vdkNkITgniHeq90bjU2i2pRr2cxhXqWVoL135h0Om1R7bKh_mAeKYyE5hTZ6OLwJMZYo7Ncg6TmQafr_wC5wNM2ik6BbTg_0rLW30y3RWm4C5rXpSxl-Noh2KWqnQ-VkdUzT5mWmXalLwQ2VYK0H-69A2HJAkgCD0XYqolTi4yZ4zpSi6rbj1ZBlrQmryZKzxfKjMOlHPcIp3q5Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Lendio</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Do you want to know why Lendio is an awesome place to work? It’s people like you.
+Seriously.
+As a co...</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Front End Developer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/partner/jobListing.htm?pos=104&amp;ao=1110586&amp;s=58&amp;guid=0000017d01d12a9bb5752966b9d2839f&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=8F7263A855640A9C3D929937C67FB101&amp;ea=1&amp;cs=1_20ee96cd&amp;cb=1636413025418&amp;jobListingId=1007390767161&amp;cpc=7FA2BCC6CA7CFB05&amp;jrtk=3-0-1fk0t2ambu4um801-1fk0t2amou3mo800-685f9fc3f0a39459--6NYlbfkN0D-cI4CbwC_TAQU56XrOPDqGahP51DR-c2q_sucHy2UMPSzCzo3z3qY4cJsao6z2d8UXDlLwj7Ef4GWR63MnIBvRReiCO_FSYy_zgraupYz34DYqX7STUjzzdE45RlcxUPrsurK47EyaWiBUrVbtGJtDNtYohhf1mVt2otfTy8cY6fMhgBUmEfEMxlGCpmfH0uWgbb-PRIOwH2AKksUI8qGLlpr0OK0nHtDwsdr1-GmKKr_R2Acln15gzfh_JgNPWD1aRMkMOpWlub4YuS0O-DZ9kA382nlzpoUOULDmfZlybgN5SYk_tAeeSE4dKIqWXcn8eQZirnutH3JmZwod_vTRHQqMcA6sHLnXqd0pqUj1miLNREt913GcXQXaMlboeAdVoJbdNwOp45Y8tXliCnsMHQCS-WSKdlOvGqo86SC7yyYI8SqEtM-819awwexbPNiOPu4LGhuW87-qyHxgRbarWc3tYtGWznSFcYJdon90JzhpwDL-AL2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>USIO, Inc.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ABOUT USIOUsio, Inc. (Nasdaq: USIO), a leading FinTech integrated payment solutions provider, offers...</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Front End UI/UX Software Engineer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/partner/jobListing.htm?pos=105&amp;ao=1110586&amp;s=58&amp;guid=0000017d01d12a9bb5752966b9d2839f&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=8F7263A855640A9C3D929937C67FB101&amp;cs=1_ae2b9b0d&amp;cb=1636413025416&amp;jobListingId=1007406135489&amp;cpc=43E37B7B5399EAEF&amp;jrtk=3-0-1fk0t2ambu4um801-1fk0t2amou3mo800-37a871581f2b45d2--6NYlbfkN0BqJjBsvJkVIRVupdyx-l7jJlkPL5nU6SVET5Mq4mDejcdzcnu2kZGUZ80A4U1mFZbpBUwx8fDdv6KvfcQ6Yz6nvIt3GlCoyiDdKFslGoEsd5fB6HQDKI-EhpUuY-uP2RTSleFkZx0Xp-l_ACNgS7m54rlku4yQAKe2Eszwyt3EUrwh1K7W5Bbl182ZqELupXR22lnZg5LvgnFtBdOk59IPMrYg2TeXwd7CJE0Cjz0n-AQ0MFRPwDNYbj9RkFlDncwpx6M-4W3QqqJUeQ1Wu562b7mURTDG07WUnC6nFL9DkE4t-7inIm7gFg49UFZszgcKldMZwhHBZ-KAbo580bpKkgbVJ-sT_cbtvsVEhYLmKN1g4vmXn60zzV1bemoAYnqKtXUscVTeAanaK2UNHywS-D0apTO9ycEJ644DHmi3Ya5lgKSHpFv5lsix7nuEiMOstVTb-_-5YlafRv1ufFdnlzA5ldFJWx86LStPIibaPXxcM4EZILVIvMtVEru1GElox9OW61Kv04E_m4Qk3LU2AJ6nHQV7Dyq695DWZvZqNA4UIp1A2mJ6Padnx2Qx6Js%3D</x:t>
+  </x:si>
+  <x:si>
+    <x:t>General Motors</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> N/A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Senior Software Engineering - REMOTE Opportunity</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/partner/jobListing.htm?pos=106&amp;ao=1110586&amp;s=58&amp;guid=0000017d01d12a9bb5752966b9d2839f&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=8F7263A855640A9C3D929937C67FB101&amp;cs=1_4171068b&amp;cb=1636413025416&amp;jobListingId=1007401844746&amp;cpc=F4333377EDC1BC7E&amp;jrtk=3-0-1fk0t2ambu4um801-1fk0t2amou3mo800-888389c0495054cc--6NYlbfkN0D0rL48rPbCci_0wY3XIb9EXXQGlB6yAzRM9Mx4TPvUm18lWycwrTn9H_X3uY5pHO6DjelkbDUS0Y_ldqJMyDsFaia6nlaEb1cESOqxKFpK04ahUCUXuYBUlQlV-XsZDkbygNkRyJOjnppCODaRweUv9eukeh1hNRoPnzQR-H4NwQuf83WN5jcrnyOTovjxZ5TR3FhKgHbWF_LL3RUFaR0NbOwiZYD9078xNSRe0XeFtvSMVRvKoWQkjmD3xVdLmdT6pq2Vhgjxj0ft6E4SUvYzKOE-Vw2QQBaSGE-gFkSyBxhrPefH-r8hiedldvhW8gKBRsrq6BA-fjfnL6Q8Vs-OuvKC5bbhxJHzI6PM-9kVSA_W9e_OKUDubB2ZfZnaNkH5pOBU8nduol_XrknfWHe3WO7QKZhO9j725My8h7sPXspQhlIBCjsXRPIyorw3rvSqtsCq2zikb7ZKlzQUaLYSvrFWCs21EV4EtJQHUFdC2IXDVBGu6zhnsVwB8iBSOPZJYM8q0P8d1O2l3IKwadH-0iA2w7QJUmeMN_GqNvmltBvaP9R7RUqn</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CustomInk</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Custom Ink is looking for a senior software engineer who has multiple years of experience in develop...</x:t>
   </x:si>
   <x:si>
     <x:t>Senior Mainframe Software Developer</x:t>
   </x:si>
   <x:si>
-    <x:t>/partner/jobListing.htm?pos=104&amp;ao=1110586&amp;s=58&amp;guid=0000017cf3b55e24b00e722ac81ba86a&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;cs=1_30714ab6&amp;cb=1636176322884&amp;jobListingId=1007406136504&amp;cpc=965F231502A4159E&amp;jrtk=3-0-1fjpranobu4kr801-1fjpranp03oej000-82a18dcc1845ea97--6NYlbfkN0BqJjBsvJkVIRVupdyx-l7jJlkPL5nU6SVET5Mq4mDejcdzcnu2kZGUZ80A4U1mFZbpBUwx8fDdv18NxMZ1-JIeLmgpBrxHGQjs2x4gXR-Mci2eOOL2TUAQnzDPpVjtX9iYbB3IRXS51lIHXwznD-RkIjJ4hq1WvqqHBgRsEk4MbdD1j2b18lACyNSMCHvXRuwyRwAzjeKX_WnH2mC5Ir9I4-IBpnKpnAm7qV7L7aeCDX98zByhPPRUhFQm5tSCfybqB1H9RfaBswVclqtxbuuZ68ncI8zdQFUvdKkh09GVe9Ef7fKx6LAVrxJmhpl-rbY4Av3snOFEVSsK1lXR02XfXbx9jWWgnsEb3GA4I-vXqKwHgoEUE6npkWhU7FYdoVhBCqZkpjQWhu5ggKUho7lis_Gr9lKht-xOcsTvDibRYXG055nqzcs4RCCipnOHDIgbCt8nRJFkUPsJHQKK_a7eytErUAk-_ixkmhXDA8lTnPm4YEocb0AuSrV_nMLvag75UX3GAK2bEF26FqKOR3ZTwjcUVl5GgrbWrGfRir7d4JkqSUVkimuZW8DWXgcj5XU%3D</x:t>
-  </x:si>
-  <x:si>
-    <x:t>General Motors</x:t>
+    <x:t>/partner/jobListing.htm?pos=107&amp;ao=1110586&amp;s=58&amp;guid=0000017d01d12a9bb5752966b9d2839f&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=8F7263A855640A9C3D929937C67FB101&amp;cs=1_321ea66d&amp;cb=1636413025416&amp;jobListingId=1007406136504&amp;cpc=72B33A28935558B9&amp;jrtk=3-0-1fk0t2ambu4um801-1fk0t2amou3mo800-82a18dcc1845ea97--6NYlbfkN0BqJjBsvJkVIRVupdyx-l7jJlkPL5nU6SVET5Mq4mDejcdzcnu2kZGUZ80A4U1mFZbpBUwx8fDdv18NxMZ1-JIeLmgpBrxHGQjs2x4gXR-Mci2eOOL2TUAQnzDPpVjtX9iYbB3IRXS51lIHXwznD-RkIjJ4hq1WvqqHBgRsEk4MbdD1j2b18lACyNSMCHvXRuxj3ZahI71tRvryC1tnBmV4gJzodJ4HnQt5bQhs3JDqXgEN5p9mnvui1XiBSNv8hUhUErjbnxFPX-Ga-SWFdRcsepWyb2auqY6DUWSVuIxR9gKD5jEZtdF0aBfu02hBQAvKnFPzEhhiixHUsOpnvuyRxnUC0k0LwIQ80Vx2FrG2HEBBkzkWjCnFPoi9iP0no5Rwwk1xuSA4-zsWgQG5cSowldC7FLg42l5rw8FmOoMoAmRhZKJpWIeJeYs6GOH0UUSC0EyFadB_dvBZUO2J_CwNmrEaWwW0B9f8KPqCu9Ul4vYI7a_2q2M1FtCmi9PySLWnovnPN8VZXy-ovdh88fsmf83a6N12waikXL5--WRpn5dPgnoN3x5C9JgY4pJPyHo%3D</x:t>
   </x:si>
   <x:si>
     <x:t>Job Description
 This position does not require an employee to be on-site full-time to perform most ...</x:t>
   </x:si>
   <x:si>
-    <x:t>Web Developer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/partner/jobListing.htm?pos=105&amp;ao=1110586&amp;s=58&amp;guid=0000017cf3b55e24b00e722ac81ba86a&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;ea=1&amp;cs=1_19351806&amp;cb=1636176322886&amp;jobListingId=1007220496222&amp;cpc=D7FE8E303655E3F3&amp;jrtk=3-0-1fjpranobu4kr801-1fjpranp03oej000-1f03e624598c7c56--6NYlbfkN0B803KHqtEZFl1zjx0sr9b9AHQOUPBdCWdQu8UhUPBs8B1dYFF-_L7StPRO-Bu5BTQNQFKFbO0lgRb97Qmo3LXKU84gnq9bjt1FUDJxlWHaLsGPsl4EjE1-DfSzPxzKY9bFKipQhdqCbHKf1kD4eK4lT-DUOhklpS_WHCvxTOCOusYI47kG3vEeOxnydhzCWMUo3HbB8GS34ys-H44Vfbmhb137KWrS08GGz9PfWDaE7CgDTW_Ul0aq8PaCLD2zSosKh0Vkfjl7oqMOXAnNeSH6GIKlztlPRnw320HDX4AwZX9MKjoSckW50QrJGgf4Y89DHIUY06bu-03bRtORfewWltBH7YmrvmxW5NB0vL_h6td_NM8NVWlRHUzjIqN0Wxvphu5DpH8cWmf_9nFiEp_BfhhdhbhotmUSK7prqEjXqEomRs1PdDfMVlLRkusZMGV9Mw4yEjTngGAw_r-oGQlSQjArS2VA63gXWRwOBu5LB6R4_lznd7l2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Goodwill Central Texas</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/partner/jobListing.htm?pos=106&amp;ao=1110586&amp;s=58&amp;guid=0000017cf3b55e24b00e722ac81ba86a&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;cs=1_109cc31d&amp;cb=1636176322884&amp;jobListingId=1007288586496&amp;cpc=FD68938D22ED3258&amp;jrtk=3-0-1fjpranobu4kr801-1fjpranp03oej000-c707ad8aee54d49b--6NYlbfkN0AEfvaTCbEyT-QU0mB1I0G9RQ6RLW6MmY4ibAKfSb27DkVWgLbvCGilYWmviU5BJjw9ZwMYa5zvaVC20v3HXl291F_jrOcEBhjOFdEM3lH5kKSjV9BFkKBA3r4fY6aWxcaOE2JtxzLEUPMIncyAN6GgrAi6MnrRw8QozOg_d9wnjM2uT7rnFnqZxPs9CN87zunquYlNCZSYZBzyc3E9Vh-PaS5SnS31ZEDZ-UwQkjZT6I4vscf7uoQP78bFjkDsdkuY0bBnsJX6m4eOs38uRUOEjWBTuC5brhGTiLTdE2DkGKM7t4Ekg-dHHVI9IO9VLHwWIGuMO4PAQ4LRAC1OVMhVoO_ShFJFfAE_4ZU4Sla_DS0OQaNCjI0Vd4gEwUslTtxSoGr8naJ3eFEqBJeiv64xFWLWfvJH1-_Ny_JFnlhYZOgvWwm_PeywQgOvOsW_hpo2diMW6NXAQztuRbWag4pjknkb4oT1SbE6EKjgauTGb_B6WMr-bfTlkdrJRqifaWw1pSE9-7Zz6bFAZoiFWf1Pv5Y1BFC_QT5m68qiBn95jOdRnOtnd5Sa5WDOyTkhvntYw3mQOrkJKhSTXsmC29TPD55hWSgoY7bfat4gFAk3DKkrkQ8TjRWqZmuHcqi8jtYDSIaCa99Q4Q%3D%3D</x:t>
-  </x:si>
-  <x:si>
-    <x:t>The Judge Group</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Location: Austin, TX
-Description: Our client is currently seeking a Sr. Software Developer with 6+ y...</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Senior Software Developer (Web)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/partner/jobListing.htm?pos=107&amp;ao=1110586&amp;s=58&amp;guid=0000017cf3b55e24b00e722ac81ba86a&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;cs=1_59a912af&amp;cb=1636176322885&amp;jobListingId=1007406136310&amp;cpc=6BDFADFCA66887C5&amp;jrtk=3-0-1fjpranobu4kr801-1fjpranp03oej000-9935c0f7a7fbadb6--6NYlbfkN0BqJjBsvJkVIRVupdyx-l7jJlkPL5nU6SVET5Mq4mDejcdzcnu2kZGUZ80A4U1mFZbpBUwx8fDdv9SCwe-a4NdmAoNbT_RjLUBx9gIM-h4lWR9gFNmgn9nRlz9z_4L3AVdmnbMhVIWuWPJ1BWd_owRoFrKY3z3x3-ZiTyGZnZaiso3Fxuc4TqAJc7VRt4AfNFxFBAH2EoeROzigvoTvBZdFU3JTsUIwt8UTt0SUMjnDpLup1S4Uh0APuI0Uzh1nZD9m97Em5fiWR9i6sYx0j8DiAMQxk2xFhrOJ0e-zWLWIm_NxQPlMn0gwqXFBhDvofqft5ZJtF0SMwTO0RM3Bjm8xaOVBQg94C9xEmOqWRwCrVMprIR8VLxGQWpX1kgru3F-cHG-XtZfZpAQlTP8Be5SLYhVOf-nWRzdKPn9_WxXlNaE03-3oAnv1ZsOS-VXVwnt9eohEVRyGIsCt3lT7X6QFw6mD_-kpdfPubqpOCyyydVXxu1aJxGxSiBioVQaSeaUgwatvAgs2ogrOpami-cdZW7yxIvkuvQSJaaqpuPt9i0ptccRRnNw_U9bzgOsdIamPq6NVdU23FnMG8kF3ceCM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Job Description
-Note, this position is:
-Hybrid: This position does not require an employee to be on...</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/partner/jobListing.htm?pos=108&amp;ao=1110586&amp;s=58&amp;guid=0000017cf3b55e24b00e722ac81ba86a&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;ea=1&amp;cs=1_877d2dcb&amp;cb=1636176322887&amp;jobListingId=1007396059475&amp;cpc=A356F292FF34F670&amp;jrtk=3-0-1fjpranobu4kr801-1fjpranp03oej000-f10c738a99eece92--6NYlbfkN0BQMpcAWCQvUn60_hvKXr45ZgFMonFQYH4GyY5XjyV3_Se_3-QvbSfxe_g8vlWm-FrYYPeETJ38AI6mY3IHlLADmzKblXkCN5YW1EUwSneadLA_3uK-YCdxxcBu-x4RlyvHL2cUiIkimDrYiqbRJHKz27OfpcBgRckBGP_m-DskMb_YbeZ2gAPrnvYh1MS_SUsxs_EUw9N2m966FGCWpD7SRkBy8Y3MJ2OhcskjFYl9UtzdICchr75YzIYs7pCE-5QMs5tpPr24AxiKAcpyLlsWZLcle_96H8NoJt6tn_NF202EwbWsXko1x34L2epwRi8YrB5DJU3IcgY7I1yZq2BNKscWSzqLeqlbNZZHdX5KBBrkDboX6-NJlArUoOpSYDnH3VuJ2k_tKfqpLfp-us6E1wjf0nmScXMbRiPyWBuFQsKdZf1yBvJXiRC46EMB7HHkqYfCFJDO2ZngnlvQpGYR4lcucJWGMFqzZ8s3YpmllW-Pz_7fCqjx</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Triller</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ABOUT TRILLER: Triller is an AI-powered music video app that allows users to create professional-loo...</x:t>
+    <x:t>Front End Developer III</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/partner/jobListing.htm?pos=108&amp;ao=1110586&amp;s=58&amp;guid=0000017d01d12a9bb5752966b9d2839f&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=8F7263A855640A9C3D929937C67FB101&amp;cs=1_b5219b2d&amp;cb=1636413025417&amp;jobListingId=1007259536303&amp;cpc=3F4BEC3597F56A5D&amp;jrtk=3-0-1fk0t2ambu4um801-1fk0t2amou3mo800-f5d321f7a14a2497--6NYlbfkN0Bvyxp-5kT5PI0anTaEYoEkcOlTMlp7z8iufLqgdrGl7itwnSg21KHIOtuVoj_q9GjQIs3UwsfWAGVx1LMfpq_M7RTu8dhakQ_72loRncYo4vtoct9EQNCh1JD6wDDcDKxR_MPT8E0DN96S4dqeGYQEkX7keSPHT6K2FNpMpNUX2SlBI2bRVVVNvYd403cptYL5HGfCjvCkU779RdCZquIaT1UvEDdW6BV657MHJWX-sD0OapuYBNF7LwUJpC98cq3e5EvOjGrPRD1Cna-roAb1tVjkfZiLHaJSEGdXgYg5Jvg0RsP0aHl6k7AC-KpqQHwRlvM7jSlof7ATcxVu2eVYJZNkvfZVMEvVaDILbdREFn5dD2ZqKgMo4qIhLi6YBT2QDDgO9kC2RpxOeZLUvkbRMRctc6Dj2-mBBJz9kN49d4_5TzJS4_K8josYgOKMgIcbi5pBDFYRQRAxGIusaFtdUvbrmwOEjoZSdgBzy4HqIE2yzxBDdOXjCXis7_z8yapJX1Sk6sKLry94dkptVSHQMZFS92p2oGSnYBu3LoYTMA%3D%3D</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Charles Schwab</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Your Opportunity
+At Schwab, we aim to transform people’s lives by changing the way the world invests...</x:t>
   </x:si>
   <x:si>
     <x:t>Senior Software Developer</x:t>
   </x:si>
   <x:si>
-    <x:t>/partner/jobListing.htm?pos=109&amp;ao=1110586&amp;s=58&amp;guid=0000017cf3b55e24b00e722ac81ba86a&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;cs=1_6615e1d5&amp;cb=1636176322885&amp;jobListingId=1007415981084&amp;cpc=EB1BD5B9C2162114&amp;jrtk=3-0-1fjpranobu4kr801-1fjpranp03oej000-6e21b099e8b54452--6NYlbfkN0BqJjBsvJkVIRVupdyx-l7jJlkPL5nU6SVET5Mq4mDejcdzcnu2kZGUZ80A4U1mFZYJv3qTHmVicbXZA5lWw6j4VkWWn6w2ZC9F86M6RU6PfZ3_6dd4Q8E5z71PSBWsoM7Fu3gqK67b1kOsdvYh7vizPCjkEBA5I7JFOK3MIv7Ro70y46opsOXPXHI7DML3_ZpcYUjs5GEMRn-MuOZv-_1TnrHf44DQ5EYqpoa7EcU-DCRBdqThNa_E8uZ59HUT31EnSmmE2At9MrQc0xHkkuJm5MuW5g1azvsTkr7o8JCL6Mch75edan63ldLUcC_5iB7Rp73G8b3aGvckoQCD1N1YdWJUdI_QJrqYfokS0x3GKL0WHlMSl1kjzNW5hlwwj9DpEJ-fkAy_aVMcjbixjV6uzaNlShU3f8-wkwyYrpcgetlyOOWjw1A-fo-oOO_pQLflv_TsRZvMnTMrbZANny6iisdD9WyB6xhH1kv3ngt9FNwFtO6KLOh4TgADD_MzwWnQujwyYlRA-riDdnBCIH88NZHuk98LXrbVLyqlYORxacIAjDK6rI07uIGIpeFMO6o%3D</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> N/A</x:t>
+    <x:t>/partner/jobListing.htm?pos=109&amp;ao=1110586&amp;s=58&amp;guid=0000017d01d12a9bb5752966b9d2839f&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=8F7263A855640A9C3D929937C67FB101&amp;cs=1_f104c631&amp;cb=1636413025417&amp;jobListingId=1007415981084&amp;cpc=66EACBD3E279A8FF&amp;jrtk=3-0-1fk0t2ambu4um801-1fk0t2amou3mo800-6e21b099e8b54452--6NYlbfkN0BqJjBsvJkVIRVupdyx-l7jJlkPL5nU6SVET5Mq4mDejcdzcnu2kZGUZ80A4U1mFZYJv3qTHmVicbXZA5lWw6j4VkWWn6w2ZC9F86M6RU6PfZ3_6dd4Q8E5z71PSBWsoM7Fu3gqK67b1kOsdvYh7vizPCjkEBA5I7JFOK3MIv7Ro70y46opsOXPXHI7DML3_ZoMtNF9JuhJP5Qd8qIhEqX8VYYADJhP1VxkNonj4IA3NZxY1Jq8izX6cV6w_uOctjv0GnGsW5K6uzwov6DHmFfU1RGJrYUyoHgiH7EJEEIOJKF1oJ74XPVbVaGlJx0-FVS3J2Z_suFyPSGp_NEopn-kMDcndvqvdhsn3Sstwq3QsoYQmqUAlwYJ1E0SLFqLvEXYlp-T15XSp65wMalXP0Hk98In7Nv8XB_D5J8nplq3isn3ex3iD75c4SEDW2L6a4uyiFuIQrohF1ezCqoMKS2KFnvp6tGmdWJWcUrH2mQDt1bLAoOTniVAwTweOHGE76QuK5GAgTAmdZ8ZQ7xpmMbjdCgVZPEMdz0Ws8JYBgX2apw0brezpN34VtbZLv3j0NA%3D</x:t>
   </x:si>
   <x:si>
     <x:t>Job Description
 This is a Hybrid position within our IT Organization. The role will allow employees...</x:t>
   </x:si>
   <x:si>
-    <x:t>Senior Software Engineering - REMOTE Opportunity</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/partner/jobListing.htm?pos=110&amp;ao=1110586&amp;s=58&amp;guid=0000017cf3b55e24b00e722ac81ba86a&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;cs=1_25cbea8c&amp;cb=1636176322886&amp;jobListingId=1007401844746&amp;cpc=5075878B7C32FFAE&amp;jrtk=3-0-1fjpranobu4kr801-1fjpranp03oej000-888389c0495054cc--6NYlbfkN0D0rL48rPbCci_0wY3XIb9EXXQGlB6yAzRM9Mx4TPvUm18lWycwrTn9H_X3uY5pHO6DjelkbDUS0Y_ldqJMyDsFaia6nlaEb1cESOqxKFpK04ahUCUXuYBUlQlV-XsZDkbygNkRyJOjnppCODaRweUv9eukeh1hNRoPnzQR-H4NwXZcYqEHWM_1qHa5Xrlt4bzIszZc4qTvhXpRWcIl7KEc7WG06iaffgx3fglZz1jnfxrY211_3CCSjT-bFXLoRznnUTV1WxwjY-LP7SxPPeAXgnj7H3gxNfuQhjbCpazNZ8eC9jf0dzfO-qTck15VSsg4X8_GhiegNNQIFxphvV4FfVs8HyIcMIm3uGUY78jZU4WXfQdGofIpFJjwxn9Gy1UfeKzhyEaa9ZixEJzYvyB4haRKE5jXBQAtXyOtPCNzoEUab9bYz9zaOWKrD_uB29GodntlX33v-kFw3NHc3kxxYomv1mJ1BdwyWVjUkquPnZL28X66biHiH0DiqSXWDZ2MqVNzr9XuAijSwYpgXa5amTliRjBrCe5Ixm8GwKruCcQ9f1vGPJRf</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CustomInk</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Custom Ink is looking for a senior software engineer who has multiple years of experience in develop...</x:t>
+    <x:t>Senior Software Engineer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/partner/jobListing.htm?pos=110&amp;ao=1110586&amp;s=58&amp;guid=0000017d01d12a9bb5752966b9d2839f&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=8F7263A855640A9C3D929937C67FB101&amp;ea=1&amp;cs=1_cda24f54&amp;cb=1636413025420&amp;jobListingId=1007201919061&amp;cpc=63C68CF611DF075E&amp;jrtk=3-0-1fk0t2ambu4um801-1fk0t2amou3mo800-34f268edad80901b--6NYlbfkN0CiRNM7CVr8YueLFKlzwbFWI0o7IjV438l4sVrvKZ0flkywQJjHRBleObb6D711Mbm5u16X-Tl1WEe_eMrpLWuHCU3aN4ot2hMTi4pud-DP1H6GmJDzYs8SLgXWQYF-uDdDqvskAvczhk4W4sbvtpiVEvqbjhWgxvvwXMGynfoTs3y6cRn_x1oGAXiVh6Nz3Ts4biDr7chp5Trxn5QhulXjyttKjcrprfHu-FXg5268TFMN9WOVGdOw06luS3pu2FgCTuIIHcljoBk6PDXRhJVjZRjAdNj5IOckAs-22CxgeqPPpHigjRMpoGO4CO_7eMk1dimS_50DZ8FrHbj_zwXO2Rwva1OkkCU8ZpARIcLXlKBHrBwgh_TDGrJKOjW6fzMx2WCUhUt1GkR48SUVo9_FevNozaKGiqCj_xOmS29zwh6fSBYXv5j4mu_gm-mnKiqzqgB0CXhy8xPxJPZOAyVm6Xb-FDyq0fmOYoODUACjTTqLRJqMUodpYrLDGfB94StvZlxa0TSiAg%3D%3D</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Indeed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Your Job
+Indeed is looking for talented and engaged engineers to join a team building out a world-cl...</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -569,7 +572,7 @@
   </x:sheetPr>
   <x:dimension ref="A1:F11"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <x:sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <x:selection activeCell="E2" sqref="E2 E2:E2"/>
     </x:sheetView>
   </x:sheetViews>
@@ -580,7 +583,7 @@
     <x:col min="3" max="3" width="32.140625" style="3" customWidth="1"/>
     <x:col min="4" max="4" width="33" style="3" customWidth="1"/>
     <x:col min="5" max="5" width="98.285156" style="3" customWidth="1"/>
-    <x:col min="6" max="6" width="99.425781" style="3" customWidth="1"/>
+    <x:col min="6" max="6" width="111.855469" style="3" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -654,24 +657,24 @@
         <x:v>19</x:v>
       </x:c>
       <x:c r="D4" s="3" t="s">
-        <x:v>20</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="E4" s="3" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="F4" s="3" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A5" s="3" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B5" s="3" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="B5" s="3" t="s">
+      <x:c r="C5" s="3" t="s">
         <x:v>23</x:v>
-      </x:c>
-      <x:c r="C5" s="3" t="s">
-        <x:v>24</x:v>
       </x:c>
       <x:c r="D5" s="3" t="s">
         <x:v>9</x:v>
@@ -680,58 +683,58 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="F5" s="3" t="s">
-        <x:v>25</x:v>
+        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A6" s="3" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="B6" s="3" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="B6" s="3" t="s">
+      <x:c r="C6" s="3" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="C6" s="3" t="s">
+      <x:c r="D6" s="3" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E6" s="3" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="D6" s="3" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="E6" s="3" t="s">
-        <x:v>10</x:v>
-      </x:c>
       <x:c r="F6" s="3" t="s">
-        <x:v>25</x:v>
+        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A7" s="3" t="s">
-        <x:v>17</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="B7" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="C7" s="3" t="s">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D7" s="3" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="E7" s="3" t="s">
-        <x:v>15</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="F7" s="3" t="s">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A8" s="3" t="s">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="B8" s="3" t="s">
-        <x:v>33</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="C8" s="3" t="s">
-        <x:v>24</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="D8" s="3" t="s">
         <x:v>9</x:v>
@@ -740,58 +743,58 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="F8" s="3" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A9" s="3" t="s">
-        <x:v>26</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="B9" s="3" t="s">
-        <x:v>35</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="C9" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="D9" s="3" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="E9" s="3" t="s">
-        <x:v>10</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="F9" s="3" t="s">
-        <x:v>37</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A10" s="3" t="s">
-        <x:v>38</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="B10" s="3" t="s">
-        <x:v>39</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="C10" s="3" t="s">
-        <x:v>24</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="D10" s="3" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="E10" s="3" t="s">
-        <x:v>40</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="F10" s="3" t="s">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A11" s="3" t="s">
-        <x:v>42</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="B11" s="3" t="s">
-        <x:v>43</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="C11" s="3" t="s">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="D11" s="3" t="s">
         <x:v>9</x:v>
@@ -800,7 +803,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="F11" s="3" t="s">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>